<commit_message>
Added more graphs and tables for keywords
</commit_message>
<xml_diff>
--- a/out/Tabelle_keywords_Anhang.xlsx
+++ b/out/Tabelle_keywords_Anhang.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paula/afd/out/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71DBFF58-58DA-F24E-806C-CDBFC1BCF8A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4DA01594-8397-414C-861B-09D08904091B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="740" windowWidth="28240" windowHeight="16840"/>
+    <workbookView xWindow="580" yWindow="740" windowWidth="28240" windowHeight="16840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="keywords_big" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="163" uniqueCount="88">
   <si>
-    <t>Word</t>
-  </si>
-  <si>
     <t>WordCount</t>
   </si>
   <si>
@@ -45,9 +42,6 @@
     <t>migration</t>
   </si>
   <si>
-    <t>1_Flucht</t>
-  </si>
-  <si>
     <t>afrika</t>
   </si>
   <si>
@@ -66,9 +60,6 @@
     <t>islamistisch</t>
   </si>
   <si>
-    <t>ausl√§nder</t>
-  </si>
-  <si>
     <t>abschiebung</t>
   </si>
   <si>
@@ -99,9 +90,6 @@
     <t>fremd</t>
   </si>
   <si>
-    <t>gef√§hrder</t>
-  </si>
-  <si>
     <t>welle</t>
   </si>
   <si>
@@ -117,9 +105,6 @@
     <t>grenzkontrolle</t>
   </si>
   <si>
-    <t>grenz√∂ffnung</t>
-  </si>
-  <si>
     <t>syrer</t>
   </si>
   <si>
@@ -132,9 +117,6 @@
     <t>eltern</t>
   </si>
   <si>
-    <t>2_Familie</t>
-  </si>
-  <si>
     <t>geschlecht</t>
   </si>
   <si>
@@ -168,9 +150,6 @@
     <t>benachteiligung</t>
   </si>
   <si>
-    <t>m√ºtter</t>
-  </si>
-  <si>
     <t>kindergarten</t>
   </si>
   <si>
@@ -240,9 +219,6 @@
     <t>impfung</t>
   </si>
   <si>
-    <t>coronama√ünahmen</t>
-  </si>
-  <si>
     <t>widerstand</t>
   </si>
   <si>
@@ -279,9 +255,6 @@
     <t>jude</t>
   </si>
   <si>
-    <t>j√ºdisch</t>
-  </si>
-  <si>
     <t>stolz</t>
   </si>
   <si>
@@ -289,12 +262,39 @@
   </si>
   <si>
     <t>linksextrem</t>
+  </si>
+  <si>
+    <t>Wort</t>
+  </si>
+  <si>
+    <t>1_Flucht_Migration</t>
+  </si>
+  <si>
+    <t>2_Familie_Gender</t>
+  </si>
+  <si>
+    <t>ausländer</t>
+  </si>
+  <si>
+    <t>gefährder</t>
+  </si>
+  <si>
+    <t>grenzöffnung</t>
+  </si>
+  <si>
+    <t>mütter</t>
+  </si>
+  <si>
+    <t>coronamaßnahmen</t>
+  </si>
+  <si>
+    <t>jüdisch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1148,30 +1148,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A80"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1179,7 +1179,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>306</v>
@@ -1191,7 +1191,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1199,7 +1199,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>301</v>
@@ -1211,7 +1211,7 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1219,7 +1219,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>297</v>
@@ -1231,7 +1231,7 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1239,7 +1239,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>243</v>
@@ -1251,7 +1251,7 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1259,7 +1259,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>173</v>
@@ -1271,7 +1271,7 @@
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1279,7 +1279,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>160</v>
@@ -1291,7 +1291,7 @@
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1299,7 +1299,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <v>135</v>
@@ -1311,7 +1311,7 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1319,7 +1319,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="C9">
         <v>128</v>
@@ -1331,7 +1331,7 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1339,7 +1339,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <v>116</v>
@@ -1351,7 +1351,7 @@
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1359,7 +1359,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C11">
         <v>100</v>
@@ -1371,7 +1371,7 @@
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1379,7 +1379,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C12">
         <v>91</v>
@@ -1391,7 +1391,7 @@
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1399,7 +1399,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>90</v>
@@ -1411,7 +1411,7 @@
         <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1419,7 +1419,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C14">
         <v>85</v>
@@ -1431,7 +1431,7 @@
         <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1439,7 +1439,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C15">
         <v>83</v>
@@ -1451,7 +1451,7 @@
         <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1459,7 +1459,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C16">
         <v>83</v>
@@ -1471,7 +1471,7 @@
         <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1479,7 +1479,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <v>77</v>
@@ -1491,7 +1491,7 @@
         <v>16</v>
       </c>
       <c r="F17" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1499,7 +1499,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C18">
         <v>76</v>
@@ -1511,7 +1511,7 @@
         <v>17</v>
       </c>
       <c r="F18" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1519,7 +1519,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C19">
         <v>72</v>
@@ -1531,7 +1531,7 @@
         <v>18</v>
       </c>
       <c r="F19" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1539,7 +1539,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="C20">
         <v>70</v>
@@ -1551,7 +1551,7 @@
         <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1559,7 +1559,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C21">
         <v>65</v>
@@ -1571,7 +1571,7 @@
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1579,7 +1579,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C22">
         <v>63</v>
@@ -1591,7 +1591,7 @@
         <v>21</v>
       </c>
       <c r="F22" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1599,7 +1599,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C23">
         <v>55</v>
@@ -1611,7 +1611,7 @@
         <v>22</v>
       </c>
       <c r="F23" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1619,7 +1619,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C24">
         <v>51</v>
@@ -1631,7 +1631,7 @@
         <v>23</v>
       </c>
       <c r="F24" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1639,7 +1639,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C25">
         <v>40</v>
@@ -1651,7 +1651,7 @@
         <v>24</v>
       </c>
       <c r="F25" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1659,7 +1659,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="C26">
         <v>39</v>
@@ -1671,7 +1671,7 @@
         <v>25</v>
       </c>
       <c r="F26" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1679,7 +1679,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C27">
         <v>38</v>
@@ -1691,7 +1691,7 @@
         <v>26</v>
       </c>
       <c r="F27" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1699,7 +1699,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C28">
         <v>37</v>
@@ -1711,7 +1711,7 @@
         <v>27</v>
       </c>
       <c r="F28" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1719,7 +1719,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C29">
         <v>29</v>
@@ -1731,7 +1731,7 @@
         <v>28</v>
       </c>
       <c r="F29" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1739,7 +1739,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C30">
         <v>304</v>
@@ -1751,7 +1751,7 @@
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1759,7 +1759,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C31">
         <v>137</v>
@@ -1771,7 +1771,7 @@
         <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1779,7 +1779,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C32">
         <v>123</v>
@@ -1791,7 +1791,7 @@
         <v>3</v>
       </c>
       <c r="F32" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1799,7 +1799,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C33">
         <v>100</v>
@@ -1811,7 +1811,7 @@
         <v>4</v>
       </c>
       <c r="F33" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1819,7 +1819,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C34">
         <v>92</v>
@@ -1831,7 +1831,7 @@
         <v>5</v>
       </c>
       <c r="F34" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1839,7 +1839,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C35">
         <v>90</v>
@@ -1851,7 +1851,7 @@
         <v>6</v>
       </c>
       <c r="F35" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1859,7 +1859,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C36">
         <v>86</v>
@@ -1871,7 +1871,7 @@
         <v>7</v>
       </c>
       <c r="F36" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1879,7 +1879,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C37">
         <v>82</v>
@@ -1891,7 +1891,7 @@
         <v>8</v>
       </c>
       <c r="F37" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1899,7 +1899,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C38">
         <v>62</v>
@@ -1911,7 +1911,7 @@
         <v>9</v>
       </c>
       <c r="F38" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1919,7 +1919,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C39">
         <v>62</v>
@@ -1931,7 +1931,7 @@
         <v>10</v>
       </c>
       <c r="F39" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -1939,7 +1939,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C40">
         <v>61</v>
@@ -1951,7 +1951,7 @@
         <v>11</v>
       </c>
       <c r="F40" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1959,7 +1959,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C41">
         <v>46</v>
@@ -1971,7 +1971,7 @@
         <v>12</v>
       </c>
       <c r="F41" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1979,7 +1979,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C42">
         <v>42</v>
@@ -1991,7 +1991,7 @@
         <v>13</v>
       </c>
       <c r="F42" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1999,7 +1999,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="C43">
         <v>35</v>
@@ -2011,7 +2011,7 @@
         <v>14</v>
       </c>
       <c r="F43" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -2019,7 +2019,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C44">
         <v>32</v>
@@ -2031,7 +2031,7 @@
         <v>15</v>
       </c>
       <c r="F44" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -2039,7 +2039,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C45">
         <v>276</v>
@@ -2051,7 +2051,7 @@
         <v>1</v>
       </c>
       <c r="F45" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -2059,7 +2059,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C46">
         <v>239</v>
@@ -2071,7 +2071,7 @@
         <v>2</v>
       </c>
       <c r="F46" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -2079,7 +2079,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C47">
         <v>230</v>
@@ -2091,7 +2091,7 @@
         <v>3</v>
       </c>
       <c r="F47" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -2099,7 +2099,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C48">
         <v>145</v>
@@ -2111,7 +2111,7 @@
         <v>4</v>
       </c>
       <c r="F48" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -2119,7 +2119,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C49">
         <v>141</v>
@@ -2131,7 +2131,7 @@
         <v>5</v>
       </c>
       <c r="F49" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -2139,7 +2139,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C50">
         <v>105</v>
@@ -2151,7 +2151,7 @@
         <v>6</v>
       </c>
       <c r="F50" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -2159,7 +2159,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C51">
         <v>90</v>
@@ -2171,7 +2171,7 @@
         <v>7</v>
       </c>
       <c r="F51" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -2179,7 +2179,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C52">
         <v>74</v>
@@ -2191,7 +2191,7 @@
         <v>8</v>
       </c>
       <c r="F52" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -2199,7 +2199,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C53">
         <v>66</v>
@@ -2211,7 +2211,7 @@
         <v>9</v>
       </c>
       <c r="F53" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -2219,7 +2219,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C54">
         <v>42</v>
@@ -2231,7 +2231,7 @@
         <v>10</v>
       </c>
       <c r="F54" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -2239,7 +2239,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C55">
         <v>36</v>
@@ -2251,7 +2251,7 @@
         <v>11</v>
       </c>
       <c r="F55" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -2259,7 +2259,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C56">
         <v>35</v>
@@ -2271,7 +2271,7 @@
         <v>12</v>
       </c>
       <c r="F56" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -2279,7 +2279,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C57">
         <v>357</v>
@@ -2291,7 +2291,7 @@
         <v>1</v>
       </c>
       <c r="F57" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -2299,7 +2299,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C58">
         <v>354</v>
@@ -2311,7 +2311,7 @@
         <v>2</v>
       </c>
       <c r="F58" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -2319,7 +2319,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C59">
         <v>169</v>
@@ -2331,7 +2331,7 @@
         <v>3</v>
       </c>
       <c r="F59" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -2339,7 +2339,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C60">
         <v>156</v>
@@ -2351,7 +2351,7 @@
         <v>4</v>
       </c>
       <c r="F60" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -2359,7 +2359,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C61">
         <v>148</v>
@@ -2371,7 +2371,7 @@
         <v>5</v>
       </c>
       <c r="F61" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -2379,7 +2379,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C62">
         <v>143</v>
@@ -2391,7 +2391,7 @@
         <v>6</v>
       </c>
       <c r="F62" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -2399,7 +2399,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C63">
         <v>140</v>
@@ -2411,7 +2411,7 @@
         <v>7</v>
       </c>
       <c r="F63" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -2419,7 +2419,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C64">
         <v>82</v>
@@ -2431,7 +2431,7 @@
         <v>8</v>
       </c>
       <c r="F64" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -2439,7 +2439,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="C65">
         <v>81</v>
@@ -2451,7 +2451,7 @@
         <v>9</v>
       </c>
       <c r="F65" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -2459,7 +2459,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C66">
         <v>74</v>
@@ -2471,7 +2471,7 @@
         <v>10</v>
       </c>
       <c r="F66" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -2479,7 +2479,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C67">
         <v>73</v>
@@ -2491,7 +2491,7 @@
         <v>11</v>
       </c>
       <c r="F67" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -2499,7 +2499,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C68">
         <v>65</v>
@@ -2511,7 +2511,7 @@
         <v>12</v>
       </c>
       <c r="F68" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -2519,7 +2519,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C69">
         <v>47</v>
@@ -2531,7 +2531,7 @@
         <v>13</v>
       </c>
       <c r="F69" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -2539,7 +2539,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C70">
         <v>47</v>
@@ -2551,7 +2551,7 @@
         <v>14</v>
       </c>
       <c r="F70" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -2559,7 +2559,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C71">
         <v>45</v>
@@ -2571,7 +2571,7 @@
         <v>15</v>
       </c>
       <c r="F71" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -2579,7 +2579,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C72">
         <v>42</v>
@@ -2591,7 +2591,7 @@
         <v>16</v>
       </c>
       <c r="F72" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -2599,7 +2599,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C73">
         <v>41</v>
@@ -2611,7 +2611,7 @@
         <v>17</v>
       </c>
       <c r="F73" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -2619,7 +2619,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C74">
         <v>38</v>
@@ -2631,7 +2631,7 @@
         <v>18</v>
       </c>
       <c r="F74" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -2639,7 +2639,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C75">
         <v>81</v>
@@ -2651,7 +2651,7 @@
         <v>1</v>
       </c>
       <c r="F75" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -2659,7 +2659,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C76">
         <v>76</v>
@@ -2671,7 +2671,7 @@
         <v>2</v>
       </c>
       <c r="F76" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -2679,7 +2679,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C77">
         <v>70</v>
@@ -2691,7 +2691,7 @@
         <v>3</v>
       </c>
       <c r="F77" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -2699,7 +2699,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C78">
         <v>61</v>
@@ -2711,7 +2711,7 @@
         <v>4</v>
       </c>
       <c r="F78" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -2719,7 +2719,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C79">
         <v>51</v>
@@ -2731,7 +2731,7 @@
         <v>5</v>
       </c>
       <c r="F79" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -2739,7 +2739,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C80">
         <v>42</v>
@@ -2751,7 +2751,7 @@
         <v>6</v>
       </c>
       <c r="F80" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>